<commit_message>
added curve for low value inductors. It's less accurate, but better than nothing.
</commit_message>
<xml_diff>
--- a/Calibration.xlsx
+++ b/Calibration.xlsx
@@ -53,8 +53,9 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -119,7 +120,7 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr bwMode="auto">
             <a:prstGeom prst="rect">
@@ -127,7 +128,7 @@
             </a:prstGeom>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:tint val="100000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -139,18 +140,88 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:f>Sheet1!$B$2:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="0"/>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$25</c:f>
+              <c:f>Sheet1!$C$2:$C$24</c:f>
               <c:numCache>
-                <c:ptCount val="24"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
                 <c:pt idx="0" formatCode="0">
                   <c:v>3059.6666666666665</c:v>
                 </c:pt>
@@ -188,45 +259,41 @@
                   <c:v>2408.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0">
-                  <c:v>2461</c:v>
+                  <c:v>2191.8333333333335</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0">
-                  <c:v>2191.8333333333335</c:v>
+                  <c:v>1992.1666666666667</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0">
-                  <c:v>1992.1666666666667</c:v>
+                  <c:v>1722.1666666666667</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0">
-                  <c:v>1722.1666666666667</c:v>
+                  <c:v>1541</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0">
-                  <c:v>1541</c:v>
+                  <c:v>1237.888888888889</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0">
-                  <c:v>1237.888888888889</c:v>
+                  <c:v>1008</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0">
-                  <c:v>1008</c:v>
+                  <c:v>770</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0">
-                  <c:v>770</c:v>
+                  <c:v>696.6666666666666</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
-                  <c:v>696.6666666666666</c:v>
+                  <c:v>514</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>514</c:v>
+                  <c:v>572</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0">
-                  <c:v>572</c:v>
-                </c:pt>
-                <c:pt idx="23" formatCode="0">
                   <c:v>553.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showBubbleSize val="0"/>
@@ -238,11 +305,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1006"/>
-        <c:axId val="1007"/>
+        <c:axId val="1012"/>
+        <c:axId val="1013"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1006"/>
+        <c:axId val="1012"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -282,7 +349,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1007"/>
+        <c:crossAx val="1013"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -290,7 +357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1007"/>
+        <c:axId val="1013"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,7 +408,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006"/>
+        <c:crossAx val="1012"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -391,7 +458,7 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="152399" y="5043487"/>
+      <a:off x="800099" y="4867274"/>
       <a:ext cx="4552949" cy="2724149"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
@@ -431,15 +498,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -450,7 +517,7 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="152399" y="5043487"/>
+        <a:off x="800099" y="4867274"/>
         <a:ext cx="4552949" cy="2724149"/>
       </xdr:xfrm>
       <a:graphic>
@@ -963,130 +1030,127 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="21.8671875"/>
-    <col bestFit="1" min="2" max="2" style="1" width="22.66796875"/>
+    <col bestFit="1" min="2" max="2" width="21.8671875"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="22.66796875"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1" t="e">
         <f>SUM(C18:E18)/3</f>
-        <v>1541</v>
-      </c>
-      <c r="C2">
+        <v>#REF!</v>
+      </c>
+      <c r="D2">
         <v>3059</v>
-      </c>
-      <c r="D2">
-        <v>3060</v>
       </c>
       <c r="E2">
         <v>3060</v>
       </c>
+      <c r="F2">
+        <v>3060</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3">
+      <c r="B3">
         <v>0.27000000000000002</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1" t="e">
         <f>SUM(C21:E21)/3</f>
-        <v>777.33333333333337</v>
-      </c>
-      <c r="C3">
+        <v>#REF!</v>
+      </c>
+      <c r="D3">
         <v>3048</v>
-      </c>
-      <c r="D3">
-        <v>3050</v>
       </c>
       <c r="E3">
         <v>3050</v>
       </c>
+      <c r="F3">
+        <v>3050</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4">
+      <c r="B4">
         <v>0.56000000000000005</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1" t="e">
         <f>SUM(C22:E22)/3</f>
-        <v>696.66666666666663</v>
-      </c>
-      <c r="C4">
+        <v>#REF!</v>
+      </c>
+      <c r="D4">
         <v>3037</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3039</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>3037</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <f>SUM(C25:H25)/6</f>
-        <v>369.16666666666669</v>
-      </c>
-      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>3034</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>3036</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>3035</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3031</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>3033</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>3030</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>784</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6">
+      <c r="B6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1" t="e">
         <f>SUM(C17:E17)/3</f>
-        <v>1776.6666666666667</v>
-      </c>
-      <c r="C6">
+        <v>#REF!</v>
+      </c>
+      <c r="D6">
         <v>2995</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>2985</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2990</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7">
+      <c r="B7">
         <v>2.7000000000000002</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1" t="e">
         <f>SUM(C23:E23)/3</f>
-        <v>518.66666666666663</v>
-      </c>
-      <c r="C7">
-        <v>2996</v>
+        <v>#REF!</v>
       </c>
       <c r="D7">
         <v>2996</v>
@@ -1094,440 +1158,474 @@
       <c r="E7">
         <v>2996</v>
       </c>
+      <c r="F7">
+        <v>2996</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8">
+      <c r="B8">
         <v>4.7000000000000002</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1" t="e">
         <f>SUM(C16:E16)/3</f>
-        <v>1972.3333333333333</v>
-      </c>
-      <c r="C8">
+        <v>#REF!</v>
+      </c>
+      <c r="D8">
         <v>2937</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>2924</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>2932</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9">
+      <c r="B9">
         <v>5.5999999999999996</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1" t="e">
         <f>SUM(C24:E24)/3</f>
-        <v>190.66666666666666</v>
-      </c>
-      <c r="C9">
+        <v>#REF!</v>
+      </c>
+      <c r="D9">
         <v>2915</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>2920</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>2922</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10">
+      <c r="B10">
         <v>6.7999999999999998</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1" t="e">
         <f>SUM(C15:E15)/3</f>
-        <v>2166</v>
-      </c>
-      <c r="C10">
+        <v>#REF!</v>
+      </c>
+      <c r="D10">
         <v>2896</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>2887</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2882</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11">
+      <c r="A11" t="e">
+        <f>C11/B11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1" t="e">
         <f>SUM(C13:K13)/9</f>
-        <v>802.77777777777783</v>
-      </c>
-      <c r="C11">
+        <v>#REF!</v>
+      </c>
+      <c r="D11">
         <v>2708</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>2786</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>2789</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>2825</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>2816</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>2821</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>2850</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>2852</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>2850</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12">
+        <f>C12/B12</f>
+        <v>115.31818181818181</v>
+      </c>
+      <c r="B12">
         <v>22</v>
       </c>
-      <c r="B12" s="1">
-        <f>SUM(C12:H12)/6</f>
+      <c r="C12" s="1">
+        <f>SUM(D12:I12)/6</f>
         <v>2537</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>2502</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>2522</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>2540</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>2586</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>2538</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>2534</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13">
+      <c r="A13" t="e">
+        <f>C13/B13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B13">
         <v>33</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1" t="e">
         <f>SUM(C14:E14)/3</f>
-        <v>2461</v>
-      </c>
-      <c r="C13">
+        <v>#REF!</v>
+      </c>
+      <c r="D13">
         <v>2409</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>2405</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>2411</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1">
-        <f>SUM(C20:E20)/3</f>
-        <v>1047.3333333333333</v>
-      </c>
-      <c r="C14">
-        <v>2453</v>
+      <c r="A14" t="e">
+        <f>C14/B14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B14">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="e">
+        <f>SUM(C11:H11)/6</f>
+        <v>#REF!</v>
       </c>
       <c r="D14">
-        <v>2484</v>
+        <v>2175</v>
       </c>
       <c r="E14">
-        <v>2446</v>
+        <v>2166</v>
+      </c>
+      <c r="F14">
+        <v>2157</v>
+      </c>
+      <c r="G14">
+        <v>2201</v>
+      </c>
+      <c r="H14">
+        <v>2219</v>
+      </c>
+      <c r="I14">
+        <v>2233</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15">
-        <v>47</v>
-      </c>
-      <c r="B15" s="1">
-        <f>SUM(C11:H11)/6</f>
-        <v>2790.8333333333335</v>
-      </c>
-      <c r="C15">
-        <v>2175</v>
+      <c r="A15" t="e">
+        <f>C15/B15</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B15">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="e">
+        <f>SUM(C19:H19)/6</f>
+        <v>#REF!</v>
       </c>
       <c r="D15">
-        <v>2166</v>
+        <v>1985</v>
       </c>
       <c r="E15">
-        <v>2157</v>
+        <v>1961</v>
       </c>
       <c r="F15">
-        <v>2201</v>
+        <v>1971</v>
       </c>
       <c r="G15">
-        <v>2219</v>
+        <v>2007</v>
       </c>
       <c r="H15">
-        <v>2233</v>
+        <v>2016</v>
+      </c>
+      <c r="I15">
+        <v>2013</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16">
-        <v>68</v>
-      </c>
-      <c r="B16" s="1">
-        <f>SUM(C19:H19)/6</f>
-        <v>1199.3333333333333</v>
-      </c>
-      <c r="C16">
-        <v>1985</v>
+      <c r="A16" t="e">
+        <f>C16/B16</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16" s="1" t="e">
+        <f>SUM(C10:H10)/6</f>
+        <v>#REF!</v>
       </c>
       <c r="D16">
-        <v>1961</v>
+        <v>1766</v>
       </c>
       <c r="E16">
-        <v>1971</v>
+        <v>1778</v>
       </c>
       <c r="F16">
-        <v>2007</v>
+        <v>1786</v>
       </c>
       <c r="G16">
-        <v>2016</v>
+        <v>1668</v>
       </c>
       <c r="H16">
-        <v>2013</v>
+        <v>1673</v>
+      </c>
+      <c r="I16">
+        <v>1662</v>
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17">
-        <v>100</v>
-      </c>
-      <c r="B17" s="1">
-        <f>SUM(C10:H10)/6</f>
-        <v>1444.1666666666667</v>
-      </c>
-      <c r="C17">
-        <v>1766</v>
+      <c r="A17" t="e">
+        <f>C17/B17</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B17">
+        <v>150</v>
+      </c>
+      <c r="C17" s="1" t="e">
+        <f>SUM(C6:E6)/3</f>
+        <v>#REF!</v>
       </c>
       <c r="D17">
-        <v>1778</v>
+        <v>1549</v>
       </c>
       <c r="E17">
-        <v>1786</v>
+        <v>1536</v>
       </c>
       <c r="F17">
-        <v>1668</v>
-      </c>
-      <c r="G17">
-        <v>1673</v>
-      </c>
-      <c r="H17">
-        <v>1662</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18">
-        <v>150</v>
-      </c>
-      <c r="B18" s="1">
-        <f>SUM(C6:E6)/3</f>
-        <v>2990</v>
-      </c>
-      <c r="C18">
-        <v>1549</v>
+      <c r="A18" t="e">
+        <f>C18/B18</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B18">
+        <v>220</v>
+      </c>
+      <c r="C18" s="1" t="e">
+        <f>SUM(C7:K7)/9</f>
+        <v>#REF!</v>
       </c>
       <c r="D18">
-        <v>1536</v>
+        <v>1207</v>
       </c>
       <c r="E18">
-        <v>1538</v>
+        <v>1212</v>
+      </c>
+      <c r="F18">
+        <v>1205</v>
+      </c>
+      <c r="G18">
+        <v>1237</v>
+      </c>
+      <c r="H18">
+        <v>1119</v>
+      </c>
+      <c r="I18">
+        <v>1216</v>
+      </c>
+      <c r="J18">
+        <v>1318</v>
+      </c>
+      <c r="K18">
+        <v>1315</v>
+      </c>
+      <c r="L18">
+        <v>1312</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19">
-        <v>220</v>
-      </c>
-      <c r="B19" s="1">
-        <f>SUM(C7:K7)/9</f>
-        <v>998.66666666666663</v>
-      </c>
-      <c r="C19">
-        <v>1207</v>
+      <c r="A19" t="e">
+        <f>C19/B19</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B19">
+        <v>330</v>
+      </c>
+      <c r="C19" s="1" t="e">
+        <f>SUM(C8:H8)/6</f>
+        <v>#REF!</v>
       </c>
       <c r="D19">
-        <v>1212</v>
+        <v>1033</v>
       </c>
       <c r="E19">
-        <v>1205</v>
+        <v>1052</v>
       </c>
       <c r="F19">
-        <v>1237</v>
+        <v>1057</v>
       </c>
       <c r="G19">
-        <v>1119</v>
+        <v>1008</v>
       </c>
       <c r="H19">
-        <v>1216</v>
+        <v>946</v>
       </c>
       <c r="I19">
-        <v>1318</v>
-      </c>
-      <c r="J19">
-        <v>1315</v>
-      </c>
-      <c r="K19">
-        <v>1312</v>
+        <v>952</v>
       </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20">
-        <v>330</v>
-      </c>
-      <c r="B20" s="1">
-        <f>SUM(C8:H8)/6</f>
-        <v>1465.5</v>
-      </c>
-      <c r="C20">
-        <v>1033</v>
-      </c>
-      <c r="D20">
-        <v>1052</v>
-      </c>
-      <c r="E20">
-        <v>1057</v>
-      </c>
-      <c r="F20">
-        <v>1008</v>
-      </c>
-      <c r="G20">
-        <v>946</v>
-      </c>
-      <c r="H20">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25">
-      <c r="A21">
+        <f>C20/B20</f>
+        <v>4.3023640661938538</v>
+      </c>
+      <c r="B20">
         <v>470</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C20" s="1">
         <f>SUM(C5:K5)/9</f>
         <v>2022.1111111111111</v>
       </c>
-      <c r="C21">
+      <c r="D20">
         <v>794</v>
       </c>
+      <c r="E20">
+        <v>744</v>
+      </c>
+      <c r="F20">
+        <v>794</v>
+      </c>
+      <c r="G20">
+        <v>759</v>
+      </c>
+      <c r="H20">
+        <v>766</v>
+      </c>
+      <c r="I20">
+        <v>773</v>
+      </c>
+      <c r="J20">
+        <v>763</v>
+      </c>
+      <c r="K20">
+        <v>770</v>
+      </c>
+      <c r="L20">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" t="e">
+        <f>C21/B21</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B21">
+        <v>560</v>
+      </c>
+      <c r="C21" s="1" t="e">
+        <f>SUM(C9:E9)/3</f>
+        <v>#REF!</v>
+      </c>
       <c r="D21">
-        <v>744</v>
+        <v>702</v>
       </c>
       <c r="E21">
-        <v>794</v>
+        <v>702</v>
       </c>
       <c r="F21">
-        <v>759</v>
-      </c>
-      <c r="G21">
-        <v>766</v>
-      </c>
-      <c r="H21">
-        <v>773</v>
-      </c>
-      <c r="I21">
-        <v>763</v>
-      </c>
-      <c r="J21">
-        <v>770</v>
-      </c>
-      <c r="K21">
-        <v>767</v>
+        <v>686</v>
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22">
-        <v>560</v>
-      </c>
-      <c r="B22" s="1">
-        <f>SUM(C9:E9)/3</f>
-        <v>2919</v>
-      </c>
-      <c r="C22">
-        <v>702</v>
+      <c r="B22">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="1" t="e">
+        <f>SUM(C4:H4)/6</f>
+        <v>#REF!</v>
       </c>
       <c r="D22">
-        <v>702</v>
+        <v>531</v>
       </c>
       <c r="E22">
-        <v>686</v>
+        <v>508</v>
+      </c>
+      <c r="F22">
+        <v>517</v>
+      </c>
+      <c r="G22">
+        <v>509</v>
+      </c>
+      <c r="H22">
+        <v>514</v>
+      </c>
+      <c r="I22">
+        <v>505</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23">
-        <v>1000</v>
-      </c>
-      <c r="B23" s="1">
-        <f>SUM(C4:H4)/6</f>
-        <v>1518.8333333333333</v>
-      </c>
-      <c r="C23">
-        <v>531</v>
+      <c r="B23">
+        <v>2200</v>
+      </c>
+      <c r="C23" s="1" t="e">
+        <f>C3</f>
+        <v>#REF!</v>
       </c>
       <c r="D23">
-        <v>508</v>
-      </c>
-      <c r="E23">
-        <v>517</v>
-      </c>
-      <c r="F23">
-        <v>509</v>
-      </c>
-      <c r="G23">
-        <v>514</v>
-      </c>
-      <c r="H23">
-        <v>505</v>
+        <v>572</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24">
-        <v>2200</v>
-      </c>
-      <c r="B24" s="1">
-        <f>C3</f>
-        <v>3048</v>
-      </c>
-      <c r="C24">
-        <v>572</v>
+      <c r="B24">
+        <v>10000</v>
+      </c>
+      <c r="C24" s="1" t="e">
+        <f>SUM(C2:F2)/4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D24">
+        <v>556</v>
+      </c>
+      <c r="E24">
+        <v>554</v>
+      </c>
+      <c r="F24">
+        <v>553</v>
+      </c>
+      <c r="G24">
+        <v>552</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25">
-        <v>10000</v>
-      </c>
-      <c r="B25" s="1">
-        <f>SUM(C2:F2)/4</f>
-        <v>2294.75</v>
-      </c>
-      <c r="C25">
-        <v>556</v>
-      </c>
-      <c r="D25">
-        <v>554</v>
-      </c>
-      <c r="E25">
-        <v>553</v>
-      </c>
-      <c r="F25">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="C26" s="2"/>
+    </row>
   </sheetData>
-  <sortState ref="A1:K25" columnSort="0">
-    <sortCondition sortBy="value" descending="0" ref="A1:A25"/>
+  <sortState ref="B1:L24" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="B1:B24"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>